<commit_message>
parsing metadata into different csvs implemented
</commit_message>
<xml_diff>
--- a/data/240623_growth_phenotyping/ml/combined_metadata.xlsx
+++ b/data/240623_growth_phenotyping/ml/combined_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppadmana/Library/CloudStorage/Dropbox/Code/curves/data/240623_growth_phenotyping/ml/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10F1E9-F7A2-AF44-B6F9-ECB8B825F015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0AAC70-BFED-0E45-A402-311646996415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="9" xr2:uid="{EF3B948B-6C45-6649-8A7F-5D578467D8A1}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{EF3B948B-6C45-6649-8A7F-5D578467D8A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -330,12 +330,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -359,11 +365,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A4CE23-B6A4-754F-AC69-6562E574D55D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,51 +718,43 @@
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>240623</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="D2" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>49</v>
       </c>
     </row>
@@ -768,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000F1D21-F70C-4E4C-B69A-F3A583D7BF6C}">
   <dimension ref="B3:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>